<commit_message>
Release 1.1.2 - New Head to head graph
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/eliassovikgunnarsson/streamlit/tippelaget/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0F2D620-0D09-C24C-8333-712403286B9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF954B4C-752B-9B49-A329-A46C3DCDCDE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16440" activeTab="1" xr2:uid="{5445944C-8ECF-A14C-BC6D-A3BC3CAF2CAD}"/>
+    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16440" activeTab="2" xr2:uid="{5445944C-8ECF-A14C-BC6D-A3BC3CAF2CAD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="7">
   <si>
     <t>Uke</t>
   </si>
@@ -47,13 +48,16 @@
     <t>Baseline</t>
   </si>
   <si>
-    <t>Elias</t>
-  </si>
-  <si>
     <t>Mads</t>
   </si>
   <si>
     <t>Tobias</t>
+  </si>
+  <si>
+    <t>Gameweek</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Elias </t>
   </si>
 </sst>
 </file>
@@ -405,15 +409,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C865F3B5-21D7-B84A-BA67-D3E35E70A024}">
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:C9"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -423,17 +427,8 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -443,17 +438,8 @@
       <c r="C2">
         <v>800</v>
       </c>
-      <c r="D2">
-        <v>200</v>
-      </c>
-      <c r="E2">
-        <v>200</v>
-      </c>
-      <c r="F2">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -463,17 +449,8 @@
       <c r="C3">
         <v>1000</v>
       </c>
-      <c r="D3">
-        <v>200</v>
-      </c>
-      <c r="E3">
-        <v>200</v>
-      </c>
-      <c r="F3">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -483,17 +460,8 @@
       <c r="C4">
         <v>1200</v>
       </c>
-      <c r="D4">
-        <v>200</v>
-      </c>
-      <c r="E4">
-        <v>200</v>
-      </c>
-      <c r="F4">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
@@ -503,17 +471,8 @@
       <c r="C5">
         <v>1400</v>
       </c>
-      <c r="D5">
-        <v>200</v>
-      </c>
-      <c r="E5">
-        <v>200</v>
-      </c>
-      <c r="F5">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
@@ -523,17 +482,8 @@
       <c r="C6">
         <v>2200</v>
       </c>
-      <c r="D6">
-        <v>400</v>
-      </c>
-      <c r="E6">
-        <v>400</v>
-      </c>
-      <c r="F6">
-        <v>400</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
@@ -543,17 +493,8 @@
       <c r="C7">
         <v>2400</v>
       </c>
-      <c r="D7">
-        <v>400</v>
-      </c>
-      <c r="E7">
-        <v>400</v>
-      </c>
-      <c r="F7">
-        <v>611</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7</v>
       </c>
@@ -563,17 +504,8 @@
       <c r="C8">
         <v>2600</v>
       </c>
-      <c r="D8">
-        <v>758</v>
-      </c>
-      <c r="E8">
-        <v>400</v>
-      </c>
-      <c r="F8">
-        <v>611</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>8</v>
       </c>
@@ -582,15 +514,6 @@
       </c>
       <c r="C9">
         <v>2800</v>
-      </c>
-      <c r="D9">
-        <v>758</v>
-      </c>
-      <c r="E9">
-        <v>400</v>
-      </c>
-      <c r="F9">
-        <v>611</v>
       </c>
     </row>
   </sheetData>
@@ -602,7 +525,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{93274CCA-B4A1-EC41-A449-BF1C124B6C92}">
   <dimension ref="A1:C16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
@@ -787,4 +710,84 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C53F0CC7-B270-0845-84AB-F38903ACB32E}">
+  <dimension ref="A1:E4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="125" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>0</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>211</v>
+      </c>
+      <c r="E3">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>358.25</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>600</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
fixed head to head error
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/eliassovikgunnarsson/streamlit/tippelaget/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA43E51C-771B-E048-B8F2-1ACBA88BA9B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77629416-43CE-974B-9522-6AC555FAB799}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16440" xr2:uid="{5445944C-8ECF-A14C-BC6D-A3BC3CAF2CAD}"/>
+    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16440" activeTab="2" xr2:uid="{5445944C-8ECF-A14C-BC6D-A3BC3CAF2CAD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="7">
   <si>
     <t>Uke</t>
   </si>
@@ -58,9 +58,6 @@
   </si>
   <si>
     <t xml:space="preserve">Elias </t>
-  </si>
-  <si>
-    <t>s</t>
   </si>
 </sst>
 </file>
@@ -140,8 +137,8 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{77D1F958-B43A-BB4E-B290-D9CFD030EB09}" name="Table1" displayName="Table1" ref="A1:E26" totalsRowShown="0">
-  <autoFilter ref="A1:E26" xr:uid="{77D1F958-B43A-BB4E-B290-D9CFD030EB09}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{77D1F958-B43A-BB4E-B290-D9CFD030EB09}" name="Table1" displayName="Table1" ref="A1:E10" totalsRowShown="0">
+  <autoFilter ref="A1:E10" xr:uid="{77D1F958-B43A-BB4E-B290-D9CFD030EB09}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{6B82D18C-F4C7-FD42-B159-97F80E78ABC7}" name="Gameweek"/>
     <tableColumn id="2" xr3:uid="{42E74C4D-5F35-C944-BB39-C1045FC1894F}" name="Elias "/>
@@ -452,7 +449,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C865F3B5-21D7-B84A-BA67-D3E35E70A024}">
   <dimension ref="A1:C26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="L13" sqref="L13"/>
     </sheetView>
   </sheetViews>
@@ -925,10 +922,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C53F0CC7-B270-0845-84AB-F38903ACB32E}">
-  <dimension ref="A1:L26"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView zoomScale="125" workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1074,137 +1071,6 @@
         <v>1600</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A11">
-        <v>9</v>
-      </c>
-      <c r="E11">
-        <v>1800</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A12">
-        <v>10</v>
-      </c>
-      <c r="E12">
-        <v>2000</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A13">
-        <v>11</v>
-      </c>
-      <c r="E13">
-        <v>2200</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A14">
-        <v>12</v>
-      </c>
-      <c r="E14">
-        <v>2400</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A15">
-        <v>13</v>
-      </c>
-      <c r="E15">
-        <v>2600</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A16">
-        <v>14</v>
-      </c>
-      <c r="E16">
-        <v>2800</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A17">
-        <v>15</v>
-      </c>
-      <c r="E17">
-        <v>3000</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A18">
-        <v>16</v>
-      </c>
-      <c r="E18">
-        <v>3200</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A19">
-        <v>17</v>
-      </c>
-      <c r="E19">
-        <v>3400</v>
-      </c>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A20">
-        <v>18</v>
-      </c>
-      <c r="E20">
-        <v>3600</v>
-      </c>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A21">
-        <v>19</v>
-      </c>
-      <c r="E21">
-        <v>3800</v>
-      </c>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A22">
-        <v>20</v>
-      </c>
-      <c r="E22">
-        <v>4000</v>
-      </c>
-      <c r="L22" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A23">
-        <v>21</v>
-      </c>
-      <c r="E23">
-        <v>4200</v>
-      </c>
-    </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A24">
-        <v>22</v>
-      </c>
-      <c r="E24">
-        <v>4400</v>
-      </c>
-    </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A25">
-        <v>23</v>
-      </c>
-      <c r="E25">
-        <v>4600</v>
-      </c>
-    </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A26">
-        <v>24</v>
-      </c>
-      <c r="E26">
-        <v>4800</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">

</xml_diff>